<commit_message>
The pursuit of happiness, through json metadata schema files. Part 147.
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -2524,7 +2524,7 @@
     <t xml:space="preserve">impdetallpeop</t>
   </si>
   <si>
-    <t xml:space="preserve">All Demographics</t>
+    <t xml:space="preserve">People (All Demographics)</t>
   </si>
   <si>
     <t xml:space="preserve">impdetcrop</t>
@@ -2830,7 +2830,7 @@
     <t xml:space="preserve">esttype_model</t>
   </si>
   <si>
-    <t xml:space="preserve">Modelled</t>
+    <t xml:space="preserve">Modelled (no event-specific data included)</t>
   </si>
   <si>
     <t xml:space="preserve">measunitgroups</t>
@@ -7918,8 +7918,8 @@
   </sheetPr>
   <dimension ref="A1:T2427"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1146" activeCellId="0" sqref="B1146:D1149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A444" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C485" activeCellId="0" sqref="C485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
First draft of the Montandon JSON schema done!
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6246" uniqueCount="2516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6255" uniqueCount="2523">
   <si>
     <t xml:space="preserve">list_name</t>
   </si>
@@ -7592,6 +7592,63 @@
   </si>
   <si>
     <t xml:space="preserve">Number of locations or lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spatfilesoft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spatfstantiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.tiff – standard tiff format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spatfstanshp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.shp – standard shapefile </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">format</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">spatfstangeot</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.geotiff – standard geotiff </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">format</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7600,9 +7657,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7692,6 +7749,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7765,7 +7828,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7838,14 +7901,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -7911,18 +7978,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2427"/>
+  <dimension ref="A1:T1431"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A444" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C485" activeCellId="0" sqref="C485"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1403" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1431" activeCellId="0" sqref="B1431"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.71"/>
@@ -38421,9 +38488,39 @@
       <c r="N1426" s="4"/>
     </row>
     <row r="1427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1428" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B1428" s="0" t="s">
+        <v>2517</v>
+      </c>
+      <c r="C1428" s="1" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="1429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1429" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B1429" s="18" t="s">
+        <v>2519</v>
+      </c>
+      <c r="C1429" s="1" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="1430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1430" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B1430" s="18" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C1430" s="1" t="s">
+        <v>2522</v>
+      </c>
+    </row>
     <row r="1431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -39868,8 +39965,8 @@
     <mergeCell ref="A1151:D1151"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Modifying the Montandon schema to additionally supply the user with all the necessary taxonomies
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7726" uniqueCount="3499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7751" uniqueCount="3499">
   <si>
     <t xml:space="preserve">list_name</t>
   </si>
@@ -10549,7 +10549,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -10744,12 +10744,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -10815,18 +10815,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T2868"/>
+  <dimension ref="A1:T1930"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1903" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1929" activeCellId="0" sqref="B1929"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A423" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D441" activeCellId="0" sqref="D441"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.71"/>
@@ -10839,7 +10839,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="1" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="14.43"/>
@@ -20867,7 +20867,9 @@
       <c r="D418" s="8" t="s">
         <v>810</v>
       </c>
-      <c r="E418" s="5"/>
+      <c r="E418" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F418" s="5"/>
       <c r="G418" s="5"/>
       <c r="H418" s="8"/>
@@ -20886,7 +20888,9 @@
       <c r="D419" s="8" t="s">
         <v>758</v>
       </c>
-      <c r="E419" s="5"/>
+      <c r="E419" s="5" t="s">
+        <v>749</v>
+      </c>
       <c r="F419" s="5"/>
       <c r="G419" s="5"/>
       <c r="H419" s="8"/>
@@ -20905,7 +20909,9 @@
       <c r="D420" s="8" t="s">
         <v>816</v>
       </c>
-      <c r="E420" s="5"/>
+      <c r="E420" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F420" s="5"/>
       <c r="G420" s="5"/>
       <c r="H420" s="8"/>
@@ -20924,7 +20930,9 @@
       <c r="D421" s="8" t="s">
         <v>816</v>
       </c>
-      <c r="E421" s="5"/>
+      <c r="E421" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F421" s="5"/>
       <c r="G421" s="5"/>
       <c r="H421" s="8"/>
@@ -20943,7 +20951,9 @@
       <c r="D422" s="8" t="s">
         <v>814</v>
       </c>
-      <c r="E422" s="5"/>
+      <c r="E422" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F422" s="5"/>
       <c r="G422" s="5"/>
       <c r="H422" s="8"/>
@@ -20962,7 +20972,9 @@
       <c r="D423" s="8" t="s">
         <v>814</v>
       </c>
-      <c r="E423" s="5"/>
+      <c r="E423" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F423" s="5"/>
       <c r="G423" s="5"/>
       <c r="H423" s="8"/>
@@ -20981,7 +20993,9 @@
       <c r="D424" s="8" t="s">
         <v>814</v>
       </c>
-      <c r="E424" s="5"/>
+      <c r="E424" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F424" s="5"/>
       <c r="G424" s="5"/>
       <c r="H424" s="8"/>
@@ -21000,7 +21014,9 @@
       <c r="D425" s="8" t="s">
         <v>818</v>
       </c>
-      <c r="E425" s="5"/>
+      <c r="E425" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F425" s="5"/>
       <c r="G425" s="5"/>
       <c r="H425" s="8"/>
@@ -21019,7 +21035,9 @@
       <c r="D426" s="8" t="s">
         <v>804</v>
       </c>
-      <c r="E426" s="5"/>
+      <c r="E426" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="F426" s="5"/>
       <c r="G426" s="5"/>
       <c r="H426" s="8"/>
@@ -21038,7 +21056,9 @@
       <c r="D427" s="8" t="s">
         <v>804</v>
       </c>
-      <c r="E427" s="5"/>
+      <c r="E427" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="F427" s="5"/>
       <c r="G427" s="5"/>
       <c r="H427" s="8"/>
@@ -21057,7 +21077,9 @@
       <c r="D428" s="8" t="s">
         <v>812</v>
       </c>
-      <c r="E428" s="5"/>
+      <c r="E428" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="F428" s="5"/>
       <c r="G428" s="5"/>
       <c r="H428" s="8"/>
@@ -21076,7 +21098,9 @@
       <c r="D429" s="8" t="s">
         <v>792</v>
       </c>
-      <c r="E429" s="5"/>
+      <c r="E429" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="F429" s="5"/>
       <c r="G429" s="5"/>
       <c r="H429" s="8"/>
@@ -21095,7 +21119,9 @@
       <c r="D430" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E430" s="5"/>
+      <c r="E430" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F430" s="5"/>
       <c r="G430" s="5"/>
       <c r="H430" s="8"/>
@@ -21114,7 +21140,9 @@
       <c r="D431" s="8" t="s">
         <v>796</v>
       </c>
-      <c r="E431" s="5"/>
+      <c r="E431" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="F431" s="5"/>
       <c r="G431" s="5"/>
       <c r="H431" s="8"/>
@@ -21133,7 +21161,9 @@
       <c r="D432" s="8" t="s">
         <v>798</v>
       </c>
-      <c r="E432" s="5"/>
+      <c r="E432" s="5" t="s">
+        <v>745</v>
+      </c>
       <c r="F432" s="5"/>
       <c r="G432" s="5"/>
       <c r="H432" s="8"/>
@@ -21152,7 +21182,9 @@
       <c r="D433" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E433" s="5"/>
+      <c r="E433" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F433" s="5"/>
       <c r="G433" s="5"/>
       <c r="H433" s="8"/>
@@ -21171,7 +21203,9 @@
       <c r="D434" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E434" s="5"/>
+      <c r="E434" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F434" s="5"/>
       <c r="G434" s="5"/>
       <c r="H434" s="8"/>
@@ -21190,7 +21224,9 @@
       <c r="D435" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E435" s="5"/>
+      <c r="E435" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F435" s="5"/>
       <c r="G435" s="5"/>
       <c r="H435" s="8"/>
@@ -21209,7 +21245,9 @@
       <c r="D436" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E436" s="5"/>
+      <c r="E436" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F436" s="5"/>
       <c r="G436" s="5"/>
       <c r="H436" s="8"/>
@@ -21228,7 +21266,9 @@
       <c r="D437" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="E437" s="5"/>
+      <c r="E437" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F437" s="5"/>
       <c r="G437" s="5"/>
       <c r="H437" s="8"/>
@@ -21247,7 +21287,9 @@
       <c r="D438" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="E438" s="5"/>
+      <c r="E438" s="5" t="s">
+        <v>749</v>
+      </c>
       <c r="F438" s="5"/>
       <c r="G438" s="5"/>
       <c r="H438" s="8"/>
@@ -21266,7 +21308,9 @@
       <c r="D439" s="8" t="s">
         <v>774</v>
       </c>
-      <c r="E439" s="5"/>
+      <c r="E439" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="F439" s="5"/>
       <c r="G439" s="5"/>
       <c r="H439" s="8"/>
@@ -21283,9 +21327,11 @@
         <v>868</v>
       </c>
       <c r="D440" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="E440" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="E440" s="5"/>
       <c r="F440" s="5"/>
       <c r="G440" s="5"/>
       <c r="H440" s="8"/>
@@ -21302,9 +21348,11 @@
         <v>870</v>
       </c>
       <c r="D441" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="E441" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="E441" s="5"/>
       <c r="F441" s="5"/>
       <c r="G441" s="5"/>
       <c r="H441" s="8"/>
@@ -21323,7 +21371,9 @@
       <c r="D442" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="E442" s="5"/>
+      <c r="E442" s="5" t="s">
+        <v>751</v>
+      </c>
       <c r="F442" s="5"/>
       <c r="G442" s="5"/>
       <c r="H442" s="8"/>
@@ -48335,72 +48385,28 @@
         <v>3498</v>
       </c>
     </row>
-    <row r="1930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1930" s="13"/>
-    </row>
-    <row r="1931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1931" s="13"/>
-    </row>
-    <row r="1932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1932" s="13"/>
-    </row>
-    <row r="1933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1933" s="13"/>
-    </row>
-    <row r="1934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1934" s="13"/>
-    </row>
-    <row r="1935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1935" s="13"/>
-    </row>
-    <row r="1936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1936" s="13"/>
-    </row>
-    <row r="1937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1937" s="13"/>
-    </row>
-    <row r="1938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1938" s="13"/>
-    </row>
-    <row r="1939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1939" s="13"/>
-    </row>
-    <row r="1940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1940" s="13"/>
-    </row>
-    <row r="1941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1941" s="13"/>
-    </row>
-    <row r="1942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1942" s="13"/>
-    </row>
-    <row r="1943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1943" s="13"/>
-    </row>
-    <row r="1944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1944" s="13"/>
-    </row>
-    <row r="1945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1945" s="13"/>
-    </row>
-    <row r="1946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1946" s="13"/>
-    </row>
-    <row r="1947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1947" s="13"/>
-    </row>
-    <row r="1948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1948" s="13"/>
-    </row>
-    <row r="1949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1949" s="13"/>
-    </row>
-    <row r="1950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1950" s="13"/>
-    </row>
-    <row r="1951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1951" s="13"/>
-    </row>
+    <row r="1930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -49326,8 +49332,8 @@
     <mergeCell ref="A1151:D1151"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Failing with Google Earth Engine, and added some small modifications to taxonomies to finish up the Monty data export
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -10795,8 +10795,8 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1133" activeCellId="0" sqref="B1133"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1085" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1107" activeCellId="0" sqref="G1107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Preparing the merge for the PostGIS database
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -2278,13 +2278,13 @@
     <t xml:space="preserve">expcat_pop</t>
   </si>
   <si>
-    <t xml:space="preserve">Population &amp; Demographic</t>
+    <t xml:space="preserve">Population</t>
   </si>
   <si>
     <t xml:space="preserve">expcat_phyinf</t>
   </si>
   <si>
-    <t xml:space="preserve">Physical Infrastructural Assets</t>
+    <t xml:space="preserve">Built Environment &amp; Cultural Assets</t>
   </si>
   <si>
     <t xml:space="preserve">expcat_fineco</t>
@@ -2296,7 +2296,7 @@
     <t xml:space="preserve">expcat_env</t>
   </si>
   <si>
-    <t xml:space="preserve">Environmental Assets</t>
+    <t xml:space="preserve">Environmental &amp; Ecological Assets</t>
   </si>
   <si>
     <t xml:space="preserve">expcat_other</t>
@@ -10534,7 +10534,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -10749,12 +10749,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -10820,18 +10820,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A399" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D441" activeCellId="0" sqref="D441"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A449" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C472" activeCellId="0" sqref="C472"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.71"/>
@@ -10844,7 +10844,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="1" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="14.43"/>
@@ -49164,8 +49164,8 @@
     <mergeCell ref="A1409:D1409"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
updating the Desinventar database to include the specific hazards
</commit_message>
<xml_diff>
--- a/ImpactInformationProfiles.xlsx
+++ b/ImpactInformationProfiles.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="choices" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="choices" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="appear" vbProcedure="false">#REF!</definedName>
@@ -10693,7 +10693,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -10908,12 +10908,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -10978,125 +10978,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A473" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B494" activeCellId="0" sqref="B494"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B110" activeCellId="0" sqref="B110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.71"/>
@@ -11109,7 +11003,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="15" style="1" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="14.43"/>
@@ -49937,8 +49831,8 @@
     <mergeCell ref="A1435:D1435"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>